<commit_message>
Updated: - more profound cleaning for the data cleaning project - market basket analysis
</commit_message>
<xml_diff>
--- a/data_preprocessing/donnees_achats_propre.xlsx
+++ b/data_preprocessing/donnees_achats_propre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zahor\Documents\2022-2027_Studies\2024-2027_ECE\S7\Data mining\s7_data_mining\data_preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672B6C68-CED9-4F59-B34A-E3211C76EFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7717F-5894-4690-8E9C-11D0302B107D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
   <si>
     <t>TransactionID</t>
   </si>
@@ -43,13 +43,13 @@
     <t>pain</t>
   </si>
   <si>
-    <t>boulangerie</t>
+    <t>Boulangerie</t>
   </si>
   <si>
     <t>lait</t>
   </si>
   <si>
-    <t>laitage</t>
+    <t>Laitage</t>
   </si>
   <si>
     <t>beurre</t>
@@ -58,16 +58,13 @@
     <t>tomate</t>
   </si>
   <si>
-    <t>fruits &amp; légumes</t>
-  </si>
-  <si>
-    <t>fruits et legumes</t>
-  </si>
-  <si>
-    <t>pâtes</t>
-  </si>
-  <si>
-    <t>épicerie</t>
+    <t>Fruits &amp; Légumes</t>
+  </si>
+  <si>
+    <t>pates</t>
+  </si>
+  <si>
+    <t>Epicerie</t>
   </si>
   <si>
     <t>riz</t>
@@ -76,91 +73,67 @@
     <t>yaourt</t>
   </si>
   <si>
-    <t>oeufs</t>
-  </si>
-  <si>
-    <t>œufs &amp; ovoproduits</t>
-  </si>
-  <si>
     <t>oeuf</t>
   </si>
   <si>
+    <t>Œufs &amp; Ovoproduits</t>
+  </si>
+  <si>
     <t>poulet</t>
   </si>
   <si>
-    <t>boucherie</t>
+    <t>Boucherie</t>
   </si>
   <si>
     <t>poisson</t>
   </si>
   <si>
-    <t>poissonnerie</t>
+    <t>Poissonnerie</t>
   </si>
   <si>
     <t>banane</t>
   </si>
   <si>
-    <t>bananes</t>
-  </si>
-  <si>
     <t>pomme</t>
   </si>
   <si>
-    <t>pommes</t>
-  </si>
-  <si>
-    <t>fruits/légumes</t>
-  </si>
-  <si>
     <t>concombre</t>
   </si>
   <si>
-    <t>coca-cola</t>
-  </si>
-  <si>
-    <t>boissons</t>
-  </si>
-  <si>
     <t>coca cola</t>
   </si>
   <si>
-    <t>eau minerale</t>
+    <t>Boissons</t>
   </si>
   <si>
     <t>eau  minerale</t>
   </si>
   <si>
-    <t>café</t>
-  </si>
-  <si>
-    <t>thé</t>
-  </si>
-  <si>
-    <t>chocolat</t>
+    <t>cafe</t>
+  </si>
+  <si>
+    <t>the</t>
   </si>
   <si>
     <t>choco lait</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
     <t>fromage</t>
   </si>
   <si>
-    <t>crèmerie</t>
+    <t>Cremerie</t>
   </si>
   <si>
     <t>jambon</t>
   </si>
   <si>
-    <t>charcuterie</t>
+    <t>Charcuterie</t>
   </si>
   <si>
     <t>huile d'olive</t>
   </si>
   <si>
-    <t>corn-flakes</t>
+    <t>corn flakes</t>
   </si>
   <si>
     <t>beurre demi-sel</t>
@@ -290,15 +263,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF52F223-E06A-477D-945E-77744100ACCD}" name="Table1" displayName="Table1" ref="A1:F49" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
-  <autoFilter ref="A1:F49" xr:uid="{EF52F223-E06A-477D-945E-77744100ACCD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5245B98A-7CD8-4E48-ABDB-3C3859D125FD}" name="Table1" displayName="Table1" ref="A1:F49" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="A1:F49" xr:uid="{5245B98A-7CD8-4E48-ABDB-3C3859D125FD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BC538F44-AEA3-487D-B32D-8354046A5C17}" name="TransactionID"/>
-    <tableColumn id="2" xr3:uid="{4CD17196-B9EE-4474-8889-1AA8E543D258}" name="Produit"/>
-    <tableColumn id="3" xr3:uid="{A58F87F1-9C0F-41AF-A8DC-B3C99FD0B353}" name="Quantité"/>
-    <tableColumn id="4" xr3:uid="{C7F011CD-1872-486F-AE6E-84F24C59B9B4}" name="Prix"/>
-    <tableColumn id="5" xr3:uid="{735617FD-EDF1-497E-9B93-85F2AB026236}" name="Catégorie"/>
-    <tableColumn id="6" xr3:uid="{BA64E7AF-A920-49F1-BEA7-72CC9F5140CE}" name="Date" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{BFEE0AF5-C7F8-4DC2-9D5D-E46B64F37E7F}" name="TransactionID"/>
+    <tableColumn id="2" xr3:uid="{28C96CFA-B901-4172-8230-82AE248ECDF2}" name="Produit"/>
+    <tableColumn id="3" xr3:uid="{0AFF964F-3C91-48DC-9254-8AA23DF2C8E3}" name="Quantité"/>
+    <tableColumn id="4" xr3:uid="{55479E26-24F2-49D7-840A-9378D6F93E8B}" name="Prix"/>
+    <tableColumn id="5" xr3:uid="{D06E1710-3D6C-459B-85C0-1F4BBD40073D}" name="Catégorie"/>
+    <tableColumn id="6" xr3:uid="{C09C55FF-77AE-4C55-B3F3-49057C1F2A8F}" name="Date" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -592,7 +565,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,7 +574,7 @@
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -662,7 +635,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="1">
-        <v>45901</v>
+        <v>45666</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -719,10 +692,10 @@
         <v>2.1</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1">
-        <v>45902</v>
+        <v>45697</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -730,7 +703,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -739,7 +712,7 @@
         <v>0.89</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1">
         <v>45902</v>
@@ -750,7 +723,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -759,10 +732,10 @@
         <v>0.89</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="1">
-        <v>45902</v>
+        <v>45697</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -770,7 +743,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -779,7 +752,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1">
         <v>45903</v>
@@ -790,7 +763,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -799,7 +772,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="1">
         <v>45903</v>
@@ -810,7 +783,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -830,7 +803,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -842,7 +815,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="1">
-        <v>45903</v>
+        <v>45725</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -850,7 +823,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -859,7 +832,7 @@
         <v>2.5</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="1">
         <v>45904</v>
@@ -870,7 +843,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -879,10 +852,10 @@
         <v>1.4</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="1">
-        <v>45904</v>
+        <v>45756</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -890,7 +863,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -899,7 +872,7 @@
         <v>5.99</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F15" s="1">
         <v>45904</v>
@@ -910,7 +883,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -919,7 +892,7 @@
         <v>7.5</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F16" s="1">
         <v>45904</v>
@@ -930,7 +903,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <v>7</v>
@@ -950,7 +923,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -962,7 +935,7 @@
         <v>12</v>
       </c>
       <c r="F18" s="1">
-        <v>45905</v>
+        <v>45786</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -970,7 +943,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -990,7 +963,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -999,7 +972,7 @@
         <v>0.33</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1">
         <v>45905</v>
@@ -1010,7 +983,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1030,7 +1003,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1039,7 +1012,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F22" s="1">
         <v>45906</v>
@@ -1050,7 +1023,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1059,10 +1032,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F23" s="1">
-        <v>45906</v>
+        <v>45817</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1070,7 +1043,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C24">
         <v>6</v>
@@ -1079,7 +1052,7 @@
         <v>0.6</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F24" s="1">
         <v>45906</v>
@@ -1090,7 +1063,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C25">
         <v>6</v>
@@ -1099,10 +1072,10 @@
         <v>0.6</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F25" s="1">
-        <v>45906</v>
+        <v>45817</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1110,7 +1083,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1119,7 +1092,7 @@
         <v>3.2</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F26" s="1">
         <v>45907</v>
@@ -1130,7 +1103,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -1139,10 +1112,10 @@
         <v>3.1</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F27" s="1">
-        <v>45907</v>
+        <v>45847</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1150,7 +1123,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1159,7 +1132,7 @@
         <v>2.4</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" s="1">
         <v>45907</v>
@@ -1170,7 +1143,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1179,7 +1152,7 @@
         <v>2.35</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29" s="1">
         <v>45907</v>
@@ -1190,7 +1163,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1199,7 +1172,7 @@
         <v>1.8</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F30" s="1">
         <v>45907</v>
@@ -1210,7 +1183,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1219,7 +1192,7 @@
         <v>1.75</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F31" s="1">
         <v>45907</v>
@@ -1290,7 +1263,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1299,7 +1272,7 @@
         <v>1.575</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F35" s="1">
         <v>45908</v>
@@ -1310,7 +1283,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -1319,7 +1292,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F36" s="1">
         <v>45909</v>
@@ -1339,7 +1312,7 @@
         <v>1.99</v>
       </c>
       <c r="E37" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F37" s="1">
         <v>45909</v>
@@ -1350,7 +1323,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1359,7 +1332,7 @@
         <v>3.5</v>
       </c>
       <c r="E38" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F38" s="1">
         <v>45909</v>
@@ -1370,7 +1343,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1379,7 +1352,7 @@
         <v>3.45</v>
       </c>
       <c r="E39" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F39" s="1">
         <v>45909</v>
@@ -1390,7 +1363,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1399,7 +1372,7 @@
         <v>2.9</v>
       </c>
       <c r="E40" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F40" s="1">
         <v>45910</v>
@@ -1410,7 +1383,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1419,10 +1392,10 @@
         <v>2.9</v>
       </c>
       <c r="E41" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F41" s="1">
-        <v>45910</v>
+        <v>45939</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1462,7 +1435,7 @@
         <v>9</v>
       </c>
       <c r="F43" s="1">
-        <v>45901</v>
+        <v>45666</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1470,7 +1443,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C44">
         <v>6</v>
@@ -1479,7 +1452,7 @@
         <v>0.6</v>
       </c>
       <c r="E44" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F44" s="1">
         <v>45906</v>
@@ -1490,7 +1463,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1499,7 +1472,7 @@
         <v>6.2</v>
       </c>
       <c r="E45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F45" s="1">
         <v>45911</v>
@@ -1510,7 +1483,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1519,10 +1492,10 @@
         <v>6.15</v>
       </c>
       <c r="E46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F46" s="1">
-        <v>45911</v>
+        <v>45970</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1530,7 +1503,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1539,7 +1512,7 @@
         <v>2.1</v>
       </c>
       <c r="E47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F47" s="1">
         <v>45911</v>
@@ -1550,7 +1523,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1559,7 +1532,7 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="E48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F48" s="1">
         <v>45911</v>
@@ -1570,7 +1543,7 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -1582,7 +1555,7 @@
         <v>9</v>
       </c>
       <c r="F49" s="1">
-        <v>45912</v>
+        <v>46000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>